<commit_message>
index changed to crestin
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-test-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\quotation-generator-crestin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C85178-EAE8-445A-9F83-4720D3DD59F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F716315C-6228-429C-B2F6-F0049E9FE5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Organic" sheetId="1" r:id="rId1"/>
+    <sheet name="Crestin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="180">
   <si>
     <t>CJ80E6FI</t>
   </si>
@@ -625,7 +626,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -968,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9548F3BD-78D7-4C41-AEEB-86055749FC7F}">
   <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection sqref="A1:C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2937,9 +2948,1986 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2E054B-3E56-4146-BBA6-A19BCF64843F}">
+  <dimension ref="A1:C178"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>69</v>
+      </c>
+      <c r="C71">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>82</v>
+      </c>
+      <c r="C84">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+      <c r="C87">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>88</v>
+      </c>
+      <c r="C90">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C91">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>92</v>
+      </c>
+      <c r="C94">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>95</v>
+      </c>
+      <c r="C97">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>96</v>
+      </c>
+      <c r="C98">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>99</v>
+      </c>
+      <c r="C101">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>102</v>
+      </c>
+      <c r="C104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>104</v>
+      </c>
+      <c r="C106">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>105</v>
+      </c>
+      <c r="C107">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>106</v>
+      </c>
+      <c r="C108">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>107</v>
+      </c>
+      <c r="C109">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>108</v>
+      </c>
+      <c r="C110">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>109</v>
+      </c>
+      <c r="C111">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>110</v>
+      </c>
+      <c r="C112">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>111</v>
+      </c>
+      <c r="C113">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>113</v>
+      </c>
+      <c r="C115">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>114</v>
+      </c>
+      <c r="C116">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>116</v>
+      </c>
+      <c r="C118">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>117</v>
+      </c>
+      <c r="C119">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>118</v>
+      </c>
+      <c r="C120">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>120</v>
+      </c>
+      <c r="C122">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>121</v>
+      </c>
+      <c r="C123">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>122</v>
+      </c>
+      <c r="C124">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>123</v>
+      </c>
+      <c r="C125">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>124</v>
+      </c>
+      <c r="C126">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>125</v>
+      </c>
+      <c r="C127">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>126</v>
+      </c>
+      <c r="C128">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>127</v>
+      </c>
+      <c r="C129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>128</v>
+      </c>
+      <c r="C130">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>129</v>
+      </c>
+      <c r="C131">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>130</v>
+      </c>
+      <c r="C132">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>131</v>
+      </c>
+      <c r="C133">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>132</v>
+      </c>
+      <c r="C134">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>133</v>
+      </c>
+      <c r="C135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>134</v>
+      </c>
+      <c r="C136">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>135</v>
+      </c>
+      <c r="C137">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>136</v>
+      </c>
+      <c r="C138">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>137</v>
+      </c>
+      <c r="C139">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>138</v>
+      </c>
+      <c r="C140">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>139</v>
+      </c>
+      <c r="C141">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>140</v>
+      </c>
+      <c r="C142">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>141</v>
+      </c>
+      <c r="C143">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>142</v>
+      </c>
+      <c r="C144">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>143</v>
+      </c>
+      <c r="C145">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>144</v>
+      </c>
+      <c r="C146">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>145</v>
+      </c>
+      <c r="C147">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>146</v>
+      </c>
+      <c r="C148">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>147</v>
+      </c>
+      <c r="C149">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>152</v>
+      </c>
+      <c r="C150">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>154</v>
+      </c>
+      <c r="C152">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>156</v>
+      </c>
+      <c r="C154">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>157</v>
+      </c>
+      <c r="C155">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>158</v>
+      </c>
+      <c r="C156">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>159</v>
+      </c>
+      <c r="C157">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>160</v>
+      </c>
+      <c r="C158">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>148</v>
+      </c>
+      <c r="C159">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>149</v>
+      </c>
+      <c r="C160">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>150</v>
+      </c>
+      <c r="C161">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>151</v>
+      </c>
+      <c r="C162">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>161</v>
+      </c>
+      <c r="C163">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>162</v>
+      </c>
+      <c r="C164">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>163</v>
+      </c>
+      <c r="C165">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>164</v>
+      </c>
+      <c r="C166">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>165</v>
+      </c>
+      <c r="C167">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>166</v>
+      </c>
+      <c r="C168">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>167</v>
+      </c>
+      <c r="C169">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>168</v>
+      </c>
+      <c r="C170">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171" t="s">
+        <v>169</v>
+      </c>
+      <c r="C171">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>170</v>
+      </c>
+      <c r="C172">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>171</v>
+      </c>
+      <c r="C173">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>172</v>
+      </c>
+      <c r="C174">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>173</v>
+      </c>
+      <c r="C175">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>174</v>
+      </c>
+      <c r="C176">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>175</v>
+      </c>
+      <c r="C177">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>176</v>
+      </c>
+      <c r="C178">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes in index and style to add logo
</commit_message>
<xml_diff>
--- a/discount code file.xlsx
+++ b/discount code file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\quotation-generator-crestin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F716315C-6228-429C-B2F6-F0049E9FE5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAD7A66-4460-43D1-B92B-5FE59B458C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{FAA3767C-2C83-4881-9D98-861C45EF7F91}"/>
   </bookViews>
@@ -626,17 +626,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2948,7 +2938,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2960,7 +2950,7 @@
   <dimension ref="A1:C178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2973,10 +2963,10 @@
       <c r="A1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2984,10 +2974,10 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>15</v>
       </c>
     </row>
@@ -2995,10 +2985,10 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>20</v>
       </c>
     </row>
@@ -3006,10 +2996,10 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>25</v>
       </c>
     </row>
@@ -3017,10 +3007,10 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>30</v>
       </c>
     </row>

</xml_diff>